<commit_message>
change readme and testcase
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5DCCEB-0D81-4079-B883-9754E9012534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECB52E4-3DF5-4C29-AB9A-8555472ABFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t xml:space="preserve">1) Link user to respective page </t>
   </si>
   <si>
-    <t>User at Home Content Page (Browse Collection)</t>
-  </si>
-  <si>
     <t>1) Users able to browse search for collections at browse page
 2) Users able to look at entire collection at collection page 
 3) Users able to add new items at add page</t>
@@ -70,9 +67,6 @@
     <t>User at Browse Page</t>
   </si>
   <si>
-    <t xml:space="preserve"> Browse, Collection or Add</t>
-  </si>
-  <si>
     <t>1) Clicking on dropdown</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>1) Users able to look for soap collection images, soap label name,color, country and for skin type</t>
   </si>
   <si>
-    <t>1) Clicking will link user to collection page</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) Clicking will link user to respective pages </t>
   </si>
   <si>
@@ -120,16 +111,6 @@
   </si>
   <si>
     <t>Accordian dropdown</t>
-  </si>
-  <si>
-    <t>User at Bottom Home Content Page (Browse, Collection, Add)</t>
-  </si>
-  <si>
-    <t>1) Click on tab link to
-(Home, Browse, Collection, Add)</t>
-  </si>
-  <si>
-    <t>Browse collection link</t>
   </si>
   <si>
     <t>2) Search input box field in accordian</t>
@@ -173,6 +154,25 @@
     <t>1) Click on more and it will bring users to a modal view details of the product
 eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more… 
 2) At the bottom of the modal  , users able to post their username and comments , it will appear in the review section with time posted</t>
+  </si>
+  <si>
+    <t>1) Click on tab link to
+(Home, Browse, Add)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User at Home Content Page </t>
+  </si>
+  <si>
+    <t>User at Bottom Home Content Page (Browse,  Add)</t>
+  </si>
+  <si>
+    <t>1) Clicking will link user to browse page</t>
+  </si>
+  <si>
+    <t>Browse tab link (centre browse button)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Browse or Add button link</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -660,7 +660,7 @@
     <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -670,19 +670,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -692,19 +692,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -714,103 +714,103 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -820,13 +820,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
modify readme and minor changes
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D4D06-910C-4DEB-9FA9-A6A80C8C89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2975534-67DC-4C7F-A8C9-A651F5EC46C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$D$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$D$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Test Case #</t>
   </si>
@@ -177,6 +177,15 @@
 *Refer to User at Browse Page for more information(Test Case 4)
 2) Users able to add new collections at add page
 *Refer to User at Add Page for more information(Test Case 5)</t>
+  </si>
+  <si>
+    <t>1) Clicking on Logo will link to home page</t>
+  </si>
+  <si>
+    <t>1) Link user to home page</t>
+  </si>
+  <si>
+    <t>Clicking on SoapAura Logo</t>
   </si>
 </sst>
 </file>
@@ -610,10 +619,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,183 +670,195 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="202.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
       <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13" t="s">
+    <row r="19" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
minor readme changes and test case
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2975534-67DC-4C7F-A8C9-A651F5EC46C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F2E210-2F49-42FD-A424-75DAD9815986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
   </bookViews>
@@ -102,20 +102,6 @@
 2) Validation error will show  for invalid cost input such as negative value for both min and max or max value lower than min value upon clicking on search button</t>
   </si>
   <si>
-    <t>1) Users are to fill in all fields 
-eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more…
-2) Any fields that are not filled or not filled properly, validation error will be shown below each field upon clicking on add button
-3) If no fields are filled and upon clicking on add button, validation errors will show for all fields
-4) After filling all fields , click on add button located at the bottom of modal  to add to collection</t>
-  </si>
-  <si>
-    <t>1) Users are able to edit all fields in the collection 
-eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more…
-2) Any fields that are not filled or not filled properly, validation error will be shown below each field upon clicking on update button
-3) If no fields are filled and upon clicking on update button, validation errors will show for all fields
-4) After editing , click on update located at the bottom of modal  to update the changes</t>
-  </si>
-  <si>
     <t>1) Click on more and it will bring users to a modal view details of the product
 eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more… 
 2) At the bottom of the modal  , users able to post their username and comments , it will appear in the review section with time posted</t>
@@ -186,6 +172,22 @@
   </si>
   <si>
     <t>Clicking on SoapAura Logo</t>
+  </si>
+  <si>
+    <t>1) Users are to fill in all fields 
+eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more…
+2) For oil, base and milk ingredient input fill, users are to register input value by hitting enter key after keying in value 
+3) Any fields that are not filled or not filled properly, validation error will be shown below each field upon clicking on add button
+4) If no fields are filled and upon clicking on add button, validation errors will show for all fields
+5) After filling all fields , click on add button located at the bottom of modal  to add to collection</t>
+  </si>
+  <si>
+    <t>1) Users are able to edit all fields in the collection 
+eg. Imageurl, name, email ,contact no, country origin, color, skin type, treat, ingredients, recommended usage and more…
+2) For oil, base and milk ingredient input fill, users are to register input value by hitting enter key after keying in value 
+3) Any fields that are not filled or not filled properly, validation error will be shown below each field upon clicking on update button
+4) If no fields are filled and upon clicking on update button, validation errors will show for all fields
+5) After editing , click on update located at the bottom of modal  to update the changes</t>
   </si>
 </sst>
 </file>
@@ -622,7 +624,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,28 +666,28 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -695,19 +697,19 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -717,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -745,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -781,7 +783,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -796,16 +798,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -814,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.3">
@@ -826,10 +828,10 @@
         <v>9</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -840,7 +842,7 @@
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="246.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -851,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>